<commit_message>
feat: apply asian font
</commit_message>
<xml_diff>
--- a/example/attendees_list-example.xlsx
+++ b/example/attendees_list-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\joey_workspace\2024\computer\excel2ppt-nametag-generator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F88ED5E-7126-4737-8985-C4B8185EF4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F15F123-B48C-4AAF-9911-FBE0D4809CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,75 +25,77 @@
     <t>이름</t>
   </si>
   <si>
+    <t>순장</t>
+  </si>
+  <si>
+    <t>예비순장</t>
+  </si>
+  <si>
+    <t>역할</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캠퍼스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캠퍼스 역할</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성균관대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안성식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예비순장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차승연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경희대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경기대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조용우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이종화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안예은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동남대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김서영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample Num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>아주대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>민경현</t>
-  </si>
-  <si>
-    <t>순장</t>
-  </si>
-  <si>
-    <t>예비순장</t>
-  </si>
-  <si>
-    <t>역할</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캠퍼스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캠퍼스 역할</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성균관대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안성식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예비순장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차승연</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경희대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경기대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조용우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이종화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안예은</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동남대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김서영</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sample Num</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,7 +449,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A9:XFD27"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -462,19 +464,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -483,13 +485,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2:E8" si="1">B2&amp;" "&amp;D2</f>
@@ -502,13 +504,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="4" t="str">
         <f t="shared" si="1"/>
@@ -521,13 +523,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -540,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -559,13 +561,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -578,13 +580,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -597,13 +599,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update example to anonymous
</commit_message>
<xml_diff>
--- a/example/attendees_list-example.xlsx
+++ b/example/attendees_list-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\joey_workspace\2024\computer\excel2ppt-nametag-generator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F15F123-B48C-4AAF-9911-FBE0D4809CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A46B46-B8AF-41CD-9B41-2E5DE27536C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="2265" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>이름</t>
   </si>
   <si>
-    <t>순장</t>
-  </si>
-  <si>
-    <t>예비순장</t>
-  </si>
-  <si>
     <t>역할</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -43,59 +37,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>성균관대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안성식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예비순장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차승연</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경희대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경기대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조용우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이종화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안예은</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동남대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김서영</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sample Num</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아주대</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>민경현</t>
+    <t>B대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="나눔스퀘어"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍길동1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍길동2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍길동3</t>
+  </si>
+  <si>
+    <t>홍길동4</t>
+  </si>
+  <si>
+    <t>홍길동5</t>
+  </si>
+  <si>
+    <t>홍길동6</t>
+  </si>
+  <si>
+    <t>홍길동7</t>
+  </si>
+  <si>
+    <t>멘토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멘티</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -103,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -134,6 +143,11 @@
       <name val="나눔스퀘어"/>
       <family val="2"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -449,167 +463,167 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <f t="shared" ref="A2:A8" si="0">IF(D2="순장",0,1)</f>
+        <f>IF(D2="멘토",0,1)</f>
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f t="shared" ref="E2:E8" si="1">B2&amp;" "&amp;D2</f>
-        <v>아주대 순장</v>
+        <f t="shared" ref="E2:E8" si="0">B2&amp;" "&amp;D2</f>
+        <v>A대 멘토</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="A3:A8" si="1">IF(D3="멘토",0,1)</f>
+        <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>성균관대 예비순장</v>
+        <f t="shared" si="0"/>
+        <v>C대 멘토</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>경희대 순장</v>
+        <v>D대 멘토</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>경기대 예비순장</v>
+        <v>E대 멘토</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>경기대 순장</v>
+        <f>B6&amp;" "&amp;D6</f>
+        <v>B대 멘티</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>동남대 순장</v>
+        <f>B7&amp;" "&amp;D7</f>
+        <v>D대 멘티</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>성균관대 예비순장</v>
+        <f t="shared" si="0"/>
+        <v>B대 멘티</v>
       </c>
     </row>
   </sheetData>

</xml_diff>